<commit_message>
fixed bom issue with R3
</commit_message>
<xml_diff>
--- a/3Ghz_option/Agilent_3Ghz_option.xlsx
+++ b/3Ghz_option/Agilent_3Ghz_option.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaurav\Documents\Altium\Agilent_3Ghz_option\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaurav\Documents\agilent_53131A_53132A_options\3Ghz_option\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DAC8B600-576D-4194-BC2F-81075F227799}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECAF53A-DE20-48EF-8053-3059A8B2213C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="11088" xr2:uid="{D49E8C06-C4D7-4515-A56F-485D2699F3C3}"/>
+    <workbookView xWindow="14220" yWindow="1212" windowWidth="23040" windowHeight="11880" xr2:uid="{D49E8C06-C4D7-4515-A56F-485D2699F3C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Agilent_3Ghz_option" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="82">
   <si>
     <t>Comment</t>
   </si>
@@ -114,9 +114,6 @@
     <t>Wurth Standoff</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>DRL1, DRL2, DRL3, DRL4</t>
   </si>
   <si>
@@ -126,9 +123,6 @@
     <t>9774080360</t>
   </si>
   <si>
-    <t>CONMCX001</t>
-  </si>
-  <si>
     <t>MCX Female PCB Mount Connector, Thru-Hole</t>
   </si>
   <si>
@@ -138,9 +132,6 @@
     <t>CON-MCX</t>
   </si>
   <si>
-    <t>919-382J-51P</t>
-  </si>
-  <si>
     <t>220n</t>
   </si>
   <si>
@@ -171,9 +162,6 @@
     <t>RESISTOR 0805 VALUE TO BE DETERMINED</t>
   </si>
   <si>
-    <t>R1, R6</t>
-  </si>
-  <si>
     <t>ESR10EZPJ100</t>
   </si>
   <si>
@@ -255,9 +243,6 @@
     <t>R5</t>
   </si>
   <si>
-    <t>R2, R3, R7, R8</t>
-  </si>
-  <si>
     <t>CRS2010-FX-10R0ELF</t>
   </si>
   <si>
@@ -274,6 +259,18 @@
   </si>
   <si>
     <t>33uf 20V D</t>
+  </si>
+  <si>
+    <t>R2, R7, R8</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>R1, R3</t>
   </si>
 </sst>
 </file>
@@ -657,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F483CB72-100C-4C94-8B83-8B56D9C885D0}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -694,13 +691,13 @@
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>8</v>
@@ -714,13 +711,13 @@
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>11</v>
@@ -734,13 +731,13 @@
         <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>14</v>
@@ -754,13 +751,13 @@
         <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>17</v>
@@ -771,10 +768,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>18</v>
@@ -794,13 +791,13 @@
         <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>23</v>
@@ -837,13 +834,13 @@
         <v>28</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="F9" s="3">
         <v>4</v>
@@ -851,19 +848,19 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>37</v>
+        <v>79</v>
       </c>
       <c r="F10" s="3">
         <v>1</v>
@@ -871,19 +868,19 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="F11" s="3">
         <v>4</v>
@@ -891,19 +888,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="F12" s="3">
         <v>1</v>
@@ -911,19 +908,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F13" s="3">
         <v>2</v>
@@ -931,19 +928,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F14" s="3">
         <v>1</v>
@@ -951,19 +948,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="D15" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F15" s="3">
         <v>4</v>
@@ -971,39 +968,39 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>47</v>
+        <v>79</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" s="3">
-        <v>1</v>
+        <v>79</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="F17" s="3">
         <v>1</v>
@@ -1011,61 +1008,81 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F18" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="F19" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="F20" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed BOM for R1 and R3
</commit_message>
<xml_diff>
--- a/3Ghz_option/Agilent_3Ghz_option.xlsx
+++ b/3Ghz_option/Agilent_3Ghz_option.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaurav\Documents\agilent_53131A_53132A_options\3Ghz_option\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaurav\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECAF53A-DE20-48EF-8053-3059A8B2213C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BEA0859-1B66-4E4B-8EF5-BC40869124DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14220" yWindow="1212" windowWidth="23040" windowHeight="11880" xr2:uid="{D49E8C06-C4D7-4515-A56F-485D2699F3C3}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{D49E8C06-C4D7-4515-A56F-485D2699F3C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Agilent_3Ghz_option" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="81">
   <si>
     <t>Comment</t>
   </si>
@@ -261,16 +261,13 @@
     <t>33uf 20V D</t>
   </si>
   <si>
-    <t>R2, R7, R8</t>
-  </si>
-  <si>
     <t>NC</t>
   </si>
   <si>
-    <t>R6</t>
-  </si>
-  <si>
-    <t>R1, R3</t>
+    <t>R1,R6</t>
+  </si>
+  <si>
+    <t>R2, R3, R7, R8</t>
   </si>
 </sst>
 </file>
@@ -654,15 +651,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F483CB72-100C-4C94-8B83-8B56D9C885D0}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="11.88671875" customWidth="1"/>
+    <col min="1" max="4" width="11.88671875" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
@@ -848,7 +847,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>32</v>
@@ -860,7 +859,7 @@
         <v>34</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F10" s="3">
         <v>1</v>
@@ -914,7 +913,7 @@
         <v>70</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>65</v>
@@ -954,7 +953,7 @@
         <v>46</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>47</v>
@@ -968,39 +967,39 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>65</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>79</v>
+        <v>51</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>65</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F17" s="3">
         <v>1</v>
@@ -1008,81 +1007,61 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F18" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F19" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F20" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F21" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>